<commit_message>
estudo de previsão CUB SP
</commit_message>
<xml_diff>
--- a/custos_e_orcamentos/previsao_CUB/CUB.xlsx
+++ b/custos_e_orcamentos/previsao_CUB/CUB.xlsx
@@ -51,7 +51,7 @@
     <t>Adm</t>
   </si>
   <si>
-    <t xml:space="preserve">Mao-de-obra </t>
+    <t>MO</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,7 +469,7 @@
   <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>